<commit_message>
added a bunch of models and reorganized
</commit_message>
<xml_diff>
--- a/Consumer/Coca Cola.xlsx
+++ b/Consumer/Coca Cola.xlsx
@@ -5,31 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/To Be Modeled/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Consumer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D21305-6CD9-6B49-A4AE-2E54690A4726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A10AF48-7978-1949-8E4D-0A7B42549880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Sheet 1'!$A$106</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Sheet 1'!$A$19</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Sheet 1'!$B$19:$AM$19</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Sheet 1'!$B$3:$AM$3</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Sheet 1'!$A$3</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Sheet 1'!$B$106:$AM$106</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Sheet 1'!$B$19:$AM$19</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Sheet 1'!$B$3:$AM$3</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Sheet 1'!$A$106</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Sheet 1'!$A$19</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Sheet 1'!$A$3</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Sheet 1'!$B$106:$AM$106</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -46,8 +32,45 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="160">
   <si>
     <t>INCOME STATEMENT (in mln.)</t>
   </si>
@@ -329,9 +352,6 @@
   </si>
   <si>
     <t>link</t>
-  </si>
-  <si>
-    <t>Coca Cola</t>
   </si>
   <si>
     <t>Revenue Growth YoY</t>
@@ -878,7 +898,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -942,18 +962,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -963,10 +971,6 @@
     </xf>
     <xf numFmtId="10" fontId="12" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="11" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="39" fontId="11" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -990,12 +994,6 @@
     <xf numFmtId="10" fontId="1" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1007,10 +1005,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="12" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1020,6 +1014,26 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="39" fontId="11" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="1" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2395,6 +2409,425 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+  <types>
+    <type name="_linkedentity">
+      <keyFlags>
+        <key name="%cvi">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+          <flag name="ExcludeFromCalcComparison" value="1"/>
+        </key>
+      </keyFlags>
+    </type>
+    <type name="_linkedentitycore">
+      <keyFlags>
+        <key name="%EntityServiceId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%EntitySubDomainId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%EntityCulture">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%EntityId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%IsRefreshable">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+          <flag name="ExcludeFromCalcComparison" value="1"/>
+        </key>
+        <key name="%ProviderInfo">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%DataProviderExternalLinkLogo">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%DataProviderExternalLink">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%OutdatedReason">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+          <flag name="ExcludeFromCalcComparison" value="1"/>
+        </key>
+      </keyFlags>
+    </type>
+  </types>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1wljc&amp;q=XNYS%3aKO&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>THE COCA-COLA COMPANY (XNYS:KO)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-US</v>
+    <v>a1wljc</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>67.2</v>
+    <v>54.015000000000001</v>
+    <v>0.54549999999999998</v>
+    <v>0.04</v>
+    <v>6.3689999999999992E-4</v>
+    <v>USD</v>
+    <v>The Coca-Cola Company is a beverage company. The Company's segments include Europe, Middle East and Africa; Latin America; North America; Asia Pacific; Global Ventures; and Bottling Investments. It owns or licenses and markets various beverage brands, which are grouped into categories, such as Coca-Cola; sparkling flavors; water, sports, coffee and tea; juice, dairy and plant-based beverages; and emerging beverages. It owns and markets six nonalcoholic sparkling soft drink brands, such as Coca-Cola, Sprite, Fanta, Diet Coke /Coca-Cola Light, and Coca-Cola Zero Sugar. Its water, sports, coffee and tea brands include quarius, Ayataka, BODYARMOR, Ciel, Costa, dogadan, Dasani, FUZE TEA, Georgia, glaceau smartwater, glaceau vitaminwater, Gold Peak, Powerade and others. The Company’s juice, dairy and plant-based beverages brands include AdeS, Del Valle, fairlife, innocent, Minute Maid, Minute Maid Pulpy and Simply. The Company products are available to consumers in more than 200 countries.</v>
+    <v>82500</v>
+    <v>New York Stock Exchange</v>
+    <v>XNYS</v>
+    <v>XNYS</v>
+    <v>1 Coca Cola Plz NW, ATLANTA, GA, 30313-2420 US</v>
+    <v>63.039900000000003</v>
+    <v>Beverages</v>
+    <v>Stock</v>
+    <v>45022.999828008593</v>
+    <v>0</v>
+    <v>62.38</v>
+    <v>271865000000</v>
+    <v>THE COCA-COLA COMPANY</v>
+    <v>THE COCA-COLA COMPANY</v>
+    <v>62.86</v>
+    <v>28.648700000000002</v>
+    <v>62.8</v>
+    <v>62.84</v>
+    <v>4326306000</v>
+    <v>KO</v>
+    <v>THE COCA-COLA COMPANY (XNYS:KO)</v>
+    <v>1115</v>
+    <v>14348792</v>
+    <v>1919</v>
+  </rv>
+  <rv s="2">
+    <v>1</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
+  <s t="_hyperlink">
+    <k n="Address" t="s"/>
+    <k n="Text" t="s"/>
+  </s>
+  <s t="_linkedentitycore">
+    <k n="_Display" t="spb"/>
+    <k n="_DisplayString" t="s"/>
+    <k n="_Flags" t="spb"/>
+    <k n="_Format" t="spb"/>
+    <k n="_Icon" t="s"/>
+    <k n="_SubLabel" t="spb"/>
+    <k n="%EntityCulture" t="s"/>
+    <k n="%EntityId" t="s"/>
+    <k n="%EntityServiceId"/>
+    <k n="%IsRefreshable" t="b"/>
+    <k n="%ProviderInfo" t="s"/>
+    <k n="52 week high"/>
+    <k n="52 week low"/>
+    <k n="Beta"/>
+    <k n="Change"/>
+    <k n="Change (%)"/>
+    <k n="Currency" t="s"/>
+    <k n="Description" t="s"/>
+    <k n="Employees"/>
+    <k n="Exchange" t="s"/>
+    <k n="Exchange abbreviation" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Headquarters" t="s"/>
+    <k n="High"/>
+    <k n="Industry" t="s"/>
+    <k n="Instrument type" t="s"/>
+    <k n="Last trade time"/>
+    <k n="LearnMoreOnLink" t="r"/>
+    <k n="Low"/>
+    <k n="Market cap"/>
+    <k n="Name" t="s"/>
+    <k n="Official name" t="s"/>
+    <k n="Open"/>
+    <k n="P/E"/>
+    <k n="Previous close"/>
+    <k n="Price"/>
+    <k n="Shares outstanding"/>
+    <k n="Ticker symbol" t="s"/>
+    <k n="UniqueName" t="s"/>
+    <k n="Volume"/>
+    <k n="Volume average"/>
+    <k n="Year incorporated"/>
+  </s>
+  <s t="_linkedentity">
+    <k n="%cvi" t="r"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
+<supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
+  <spbArrays count="1">
+    <a count="42">
+      <v t="s">%EntityServiceId</v>
+      <v t="s">_Format</v>
+      <v t="s">%IsRefreshable</v>
+      <v t="s">%EntityCulture</v>
+      <v t="s">%EntityId</v>
+      <v t="s">_Icon</v>
+      <v t="s">_Display</v>
+      <v t="s">Name</v>
+      <v t="s">_SubLabel</v>
+      <v t="s">Price</v>
+      <v t="s">Exchange</v>
+      <v t="s">Official name</v>
+      <v t="s">Last trade time</v>
+      <v t="s">Ticker symbol</v>
+      <v t="s">Exchange abbreviation</v>
+      <v t="s">Change</v>
+      <v t="s">Change (%)</v>
+      <v t="s">Currency</v>
+      <v t="s">Previous close</v>
+      <v t="s">Open</v>
+      <v t="s">High</v>
+      <v t="s">Low</v>
+      <v t="s">52 week high</v>
+      <v t="s">52 week low</v>
+      <v t="s">Volume</v>
+      <v t="s">Volume average</v>
+      <v t="s">Market cap</v>
+      <v t="s">Beta</v>
+      <v t="s">P/E</v>
+      <v t="s">Shares outstanding</v>
+      <v t="s">Description</v>
+      <v t="s">Employees</v>
+      <v t="s">Headquarters</v>
+      <v t="s">Industry</v>
+      <v t="s">Instrument type</v>
+      <v t="s">Year incorporated</v>
+      <v t="s">_Flags</v>
+      <v t="s">UniqueName</v>
+      <v t="s">_DisplayString</v>
+      <v t="s">LearnMoreOnLink</v>
+      <v t="s">ExchangeID</v>
+      <v t="s">%ProviderInfo</v>
+    </a>
+  </spbArrays>
+  <spbData count="5">
+    <spb s="0">
+      <v>0</v>
+      <v>Name</v>
+      <v>LearnMoreOnLink</v>
+    </spb>
+    <spb s="1">
+      <v>0</v>
+      <v>0</v>
+      <v>0</v>
+    </spb>
+    <spb s="2">
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+    </spb>
+    <spb s="3">
+      <v>1</v>
+      <v>2</v>
+      <v>2</v>
+      <v>1</v>
+      <v>3</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>4</v>
+      <v>5</v>
+      <v>6</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>7</v>
+      <v>8</v>
+      <v>9</v>
+      <v>4</v>
+    </spb>
+    <spb s="4">
+      <v>Real-Time Nasdaq Last Sale</v>
+      <v>from previous close</v>
+      <v>from previous close</v>
+      <v>Source: Nasdaq Last Sale</v>
+      <v>GMT</v>
+    </spb>
+  </spbData>
+</supportingPropertyBags>
+</file>
+
+<file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="5">
+  <s>
+    <k n="^Order" t="spba"/>
+    <k n="TitleProperty" t="s"/>
+    <k n="SubTitleProperty" t="s"/>
+  </s>
+  <s>
+    <k n="ShowInCardView" t="b"/>
+    <k n="ShowInDotNotation" t="b"/>
+    <k n="ShowInAutoComplete" t="b"/>
+  </s>
+  <s>
+    <k n="ExchangeID" t="spb"/>
+    <k n="UniqueName" t="spb"/>
+    <k n="`%ProviderInfo" t="spb"/>
+    <k n="LearnMoreOnLink" t="spb"/>
+  </s>
+  <s>
+    <k n="Low" t="i"/>
+    <k n="P/E" t="i"/>
+    <k n="Beta" t="i"/>
+    <k n="High" t="i"/>
+    <k n="Name" t="i"/>
+    <k n="Open" t="i"/>
+    <k n="Price" t="i"/>
+    <k n="Change" t="i"/>
+    <k n="Volume" t="i"/>
+    <k n="Employees" t="i"/>
+    <k n="Change (%)" t="i"/>
+    <k n="Market cap" t="i"/>
+    <k n="52 week low" t="i"/>
+    <k n="52 week high" t="i"/>
+    <k n="Previous close" t="i"/>
+    <k n="Volume average" t="i"/>
+    <k n="Last trade time" t="i"/>
+    <k n="Year incorporated" t="i"/>
+    <k n="`%EntityServiceId" t="i"/>
+    <k n="Shares outstanding" t="i"/>
+  </s>
+  <s>
+    <k n="Price" t="s"/>
+    <k n="Change" t="s"/>
+    <k n="Change (%)" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Last trade time" t="s"/>
+  </s>
+</spbStructures>
+</file>
+
+<file path=xl/richData/richStyles.xml><?xml version="1.0" encoding="utf-8"?>
+<richStyleSheet xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <dxfs count="7">
+    <x:dxf>
+      <x:numFmt numFmtId="2" formatCode="0.00"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="0" formatCode="General"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="27" formatCode="m/d/yy\ h:mm"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="14" formatCode="0.00%"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="3" formatCode="#,##0"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="1" formatCode="0"/>
+    </x:dxf>
+  </dxfs>
+  <richProperties>
+    <rPr n="NumberFormat" t="s"/>
+    <rPr n="IsTitleField" t="b"/>
+  </richProperties>
+  <richStyles>
+    <rSty dxfid="1">
+      <rpv i="0">_([$$-en-US]* #,##0.00_);_([$$-en-US]* (#,##0.00);_([$$-en-US]* "-"??_);_(@_)</rpv>
+    </rSty>
+    <rSty dxfid="5">
+      <rpv i="0">#,##0.00</rpv>
+    </rSty>
+    <rSty>
+      <rpv i="1">1</rpv>
+    </rSty>
+    <rSty dxfid="4">
+      <rpv i="0">#,##0</rpv>
+    </rSty>
+    <rSty dxfid="3"/>
+    <rSty dxfid="1">
+      <rpv i="0">_([$$-en-US]* #,##0_);_([$$-en-US]* (#,##0);_([$$-en-US]* "-"_);_(@_)</rpv>
+    </rSty>
+    <rSty dxfid="2"/>
+    <rSty dxfid="6">
+      <rpv i="0">0</rpv>
+    </rSty>
+    <rSty dxfid="0">
+      <rpv i="0">0.00</rpv>
+    </rSty>
+  </richStyles>
+</richStyleSheet>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2695,10 +3128,10 @@
   <dimension ref="A1:AV118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AK83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AT140" sqref="AT140"/>
+      <selection pane="bottomRight" activeCell="AQ99" sqref="AQ99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2709,8 +3142,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>94</v>
+      <c r="A1" s="3" t="e" vm="1">
+        <v>#VALUE!</v>
       </c>
       <c r="B1" s="8">
         <v>1985</v>
@@ -3106,21 +3539,21 @@
         <v>54054000000</v>
       </c>
       <c r="AS3" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="AT3" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="AT3" s="19" t="s">
+      <c r="AU3" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="AU3" s="19" t="s">
+      <c r="AV3" s="19" t="s">
         <v>112</v>
-      </c>
-      <c r="AV3" s="19" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:48" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="15">
@@ -3546,16 +3979,16 @@
         <v>25004000000</v>
       </c>
       <c r="AS6" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="AT6" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="AT6" s="19" t="s">
+      <c r="AU6" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="AU6" s="19" t="s">
+      <c r="AV6" s="19" t="s">
         <v>116</v>
-      </c>
-      <c r="AV6" s="19" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:48" ht="19" x14ac:dyDescent="0.25">
@@ -3814,7 +4247,7 @@
     </row>
     <row r="9" spans="1:48" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="15">
         <f>B8/B3</f>
@@ -3969,16 +4402,16 @@
         <v>0</v>
       </c>
       <c r="AS9" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="AT9" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="AT9" s="19" t="s">
+      <c r="AU9" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="AU9" s="19" t="s">
+      <c r="AV9" s="19" t="s">
         <v>99</v>
-      </c>
-      <c r="AV9" s="19" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:48" ht="19" x14ac:dyDescent="0.25">
@@ -4354,21 +4787,21 @@
         <v>12880000000</v>
       </c>
       <c r="AS12" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT12" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="AT12" s="19" t="s">
+      <c r="AU12" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="AU12" s="19" t="s">
+      <c r="AV12" s="19" t="s">
         <v>120</v>
-      </c>
-      <c r="AV12" s="19" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:48" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" s="15">
         <f>B12/B3</f>
@@ -4777,16 +5210,16 @@
         <v>14095000000</v>
       </c>
       <c r="AS15" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="AT15" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="AT15" s="19" t="s">
+      <c r="AU15" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="AU15" s="19" t="s">
+      <c r="AV15" s="19" t="s">
         <v>124</v>
-      </c>
-      <c r="AV15" s="19" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:48" ht="19" x14ac:dyDescent="0.25">
@@ -4913,15 +5346,15 @@
       </c>
       <c r="AT16" s="30">
         <f>AU101/AM3</f>
-        <v>6.2185094409822339</v>
+        <v>6.3218537810436235</v>
       </c>
       <c r="AU16" s="30">
         <f>AU101/AM28</f>
-        <v>28.025652902955354</v>
+        <v>28.491406413749736</v>
       </c>
       <c r="AV16" s="31">
         <f>AU101/AM106</f>
-        <v>28.04916928886092</v>
+        <v>28.515313614432557</v>
       </c>
     </row>
     <row r="17" spans="1:45" ht="19" x14ac:dyDescent="0.25">
@@ -5162,7 +5595,7 @@
         <v>1260000000</v>
       </c>
       <c r="AS18" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:45" ht="19" x14ac:dyDescent="0.25">
@@ -5290,7 +5723,7 @@
     </row>
     <row r="20" spans="1:45" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="15">
@@ -6396,7 +6829,7 @@
     </row>
     <row r="29" spans="1:45" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="15">
@@ -7145,7 +7578,7 @@
     </row>
     <row r="35" spans="1:39" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="22">
@@ -12535,7 +12968,7 @@
     </row>
     <row r="80" spans="1:39" ht="19" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B80" s="15" t="e">
         <f t="shared" ref="B80:AM80" si="12">B79/B3</f>
@@ -13046,10 +13479,10 @@
       <c r="AM83" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AT83" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU83" s="34"/>
+      <c r="AT83" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU83" s="63"/>
     </row>
     <row r="84" spans="1:47" ht="19" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
@@ -13169,10 +13602,10 @@
       <c r="AM84" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AT84" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="AU84" s="36"/>
+      <c r="AT84" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU84" s="65"/>
     </row>
     <row r="85" spans="1:47" ht="20" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
@@ -13293,7 +13726,7 @@
         <v>92</v>
       </c>
       <c r="AT85" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AU85" s="24">
         <f>AM17</f>
@@ -13419,7 +13852,7 @@
         <v>558000000</v>
       </c>
       <c r="AT86" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AU86" s="24">
         <f>AM56</f>
@@ -13545,7 +13978,7 @@
         <v>11018000000</v>
       </c>
       <c r="AT87" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AU87" s="24">
         <f>AM61</f>
@@ -13670,17 +14103,17 @@
       <c r="AM88" s="1">
         <v>-1484000000</v>
       </c>
-      <c r="AT88" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="AU88" s="38">
+      <c r="AT88" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="AU88" s="34">
         <f>AU85/(AU86+AU87)</f>
         <v>2.2529311093514522E-2</v>
       </c>
     </row>
     <row r="89" spans="1:47" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B89" s="15" t="e">
         <f t="shared" ref="B89:AM89" si="13">(-1*B88)/B3</f>
@@ -13835,7 +14268,7 @@
         <v>3.4508417821597991E-2</v>
       </c>
       <c r="AT89" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AU89" s="24">
         <f>AM27</f>
@@ -14086,10 +14519,10 @@
       <c r="AM91" s="1">
         <v>-3751000000</v>
       </c>
-      <c r="AT91" s="37" t="s">
-        <v>133</v>
-      </c>
-      <c r="AU91" s="38">
+      <c r="AT91" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="AU91" s="34">
         <f>AU89/AU90</f>
         <v>0.18098579496833819</v>
       </c>
@@ -14212,10 +14645,10 @@
       <c r="AM92" s="1">
         <v>4771000000</v>
       </c>
-      <c r="AT92" s="39" t="s">
-        <v>134</v>
-      </c>
-      <c r="AU92" s="40">
+      <c r="AT92" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="AU92" s="36">
         <f>AU88*(1-AU91)</f>
         <v>1.8451825815165794E-2</v>
       </c>
@@ -14338,10 +14771,10 @@
       <c r="AM93" s="1">
         <v>-684000000</v>
       </c>
-      <c r="AT93" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="AU93" s="36"/>
+      <c r="AT93" s="64" t="s">
+        <v>134</v>
+      </c>
+      <c r="AU93" s="65"/>
     </row>
     <row r="94" spans="1:47" ht="20" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
@@ -14462,9 +14895,9 @@
         <v>-763000000</v>
       </c>
       <c r="AT94" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="AU94" s="41">
+        <v>135</v>
+      </c>
+      <c r="AU94" s="37">
         <v>4.095E-2</v>
       </c>
     </row>
@@ -14586,11 +15019,12 @@
       <c r="AM95" s="1">
         <v>-4930000000</v>
       </c>
-      <c r="AT95" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="AU95" s="43">
-        <v>0.54</v>
+      <c r="AT95" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="AU95" s="58" cm="1">
+        <f t="array" ref="AU95">_FV(A1,"Beta")</f>
+        <v>0.54549999999999998</v>
       </c>
     </row>
     <row r="96" spans="1:47" ht="20" x14ac:dyDescent="0.25">
@@ -14712,9 +15146,9 @@
         <v>837000000</v>
       </c>
       <c r="AT96" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="AU96" s="41">
+        <v>137</v>
+      </c>
+      <c r="AU96" s="37">
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
@@ -14836,12 +15270,12 @@
       <c r="AM97" s="1">
         <v>-1418000000</v>
       </c>
-      <c r="AT97" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="AU97" s="40">
+      <c r="AT97" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="AU97" s="36">
         <f>(AU94)+((AU95)*(AU96-AU94))</f>
-        <v>6.4197000000000004E-2</v>
+        <v>6.4433774999999999E-2</v>
       </c>
     </row>
     <row r="98" spans="1:47" ht="19" x14ac:dyDescent="0.25">
@@ -14962,10 +15396,10 @@
       <c r="AM98" s="1">
         <v>-7616000000</v>
       </c>
-      <c r="AT98" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="AU98" s="36"/>
+      <c r="AT98" s="64" t="s">
+        <v>139</v>
+      </c>
+      <c r="AU98" s="65"/>
     </row>
     <row r="99" spans="1:47" ht="20" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
@@ -15086,7 +15520,7 @@
         <v>2877000000</v>
       </c>
       <c r="AT99" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AU99" s="24">
         <f>AU86+AU87</f>
@@ -15211,12 +15645,12 @@
       <c r="AM100" s="10">
         <v>-10250000000</v>
       </c>
-      <c r="AT100" s="37" t="s">
-        <v>142</v>
-      </c>
-      <c r="AU100" s="38">
+      <c r="AT100" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="AU100" s="34">
         <f>AU99/AU103</f>
-        <v>0.12770012752072302</v>
+        <v>0.12587536252387352</v>
       </c>
     </row>
     <row r="101" spans="1:47" ht="20" x14ac:dyDescent="0.25">
@@ -15337,12 +15771,12 @@
       <c r="AM101" s="1">
         <v>-205000000</v>
       </c>
-      <c r="AT101" s="67" t="s">
-        <v>143</v>
-      </c>
-      <c r="AU101" s="58">
-        <f>AO116*AM34</f>
-        <v>267420780000</v>
+      <c r="AT101" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="AU101" s="50" cm="1">
+        <f t="array" ref="AU101">_FV(A1,"Market cap",TRUE)</f>
+        <v>271865000000</v>
       </c>
     </row>
     <row r="102" spans="1:47" ht="20" x14ac:dyDescent="0.25">
@@ -15463,12 +15897,12 @@
       <c r="AM102" s="10">
         <v>-200000000</v>
       </c>
-      <c r="AT102" s="37" t="s">
-        <v>144</v>
-      </c>
-      <c r="AU102" s="38">
+      <c r="AT102" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="AU102" s="34">
         <f>AU101/AU103</f>
-        <v>0.87229987247927698</v>
+        <v>0.87412463747612645</v>
       </c>
     </row>
     <row r="103" spans="1:47" ht="20" x14ac:dyDescent="0.25">
@@ -15589,12 +16023,12 @@
       <c r="AM103" s="1">
         <v>10025000000</v>
       </c>
-      <c r="AT103" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="AU103" s="44">
+      <c r="AT103" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="AU103" s="38">
         <f>AU99+AU101</f>
-        <v>306569780000</v>
+        <v>311014000000</v>
       </c>
     </row>
     <row r="104" spans="1:47" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -15715,14 +16149,14 @@
       <c r="AM104" s="11">
         <v>9825000000</v>
       </c>
-      <c r="AT104" s="35" t="s">
-        <v>146</v>
-      </c>
-      <c r="AU104" s="36"/>
+      <c r="AT104" s="64" t="s">
+        <v>145</v>
+      </c>
+      <c r="AU104" s="65"/>
     </row>
     <row r="105" spans="1:47" ht="21" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B105" s="1"/>
       <c r="C105" s="15" t="e">
@@ -15880,11 +16314,11 @@
       <c r="AR105" s="15"/>
       <c r="AS105" s="15"/>
       <c r="AT105" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AU105" s="26">
         <f>(AU100*AU92)+(AU102*AU97)</f>
-        <v>5.835533542313899E-2</v>
+        <v>5.864578047680466E-2</v>
       </c>
     </row>
     <row r="106" spans="1:47" ht="19" x14ac:dyDescent="0.25">
@@ -16005,33 +16439,33 @@
       <c r="AM106" s="1">
         <v>9534000000</v>
       </c>
-      <c r="AN106" s="45">
+      <c r="AN106" s="39">
         <f>AM106*(1+$AU$106)</f>
         <v>9980308058.8583813</v>
       </c>
-      <c r="AO106" s="45">
+      <c r="AO106" s="39">
         <f t="shared" ref="AO106:AR106" si="17">AN106*(1+$AU$106)</f>
         <v>10447508805.298254</v>
       </c>
-      <c r="AP106" s="45">
+      <c r="AP106" s="39">
         <f t="shared" si="17"/>
         <v>10936580273.181463</v>
       </c>
-      <c r="AQ106" s="45">
+      <c r="AQ106" s="39">
         <f t="shared" si="17"/>
         <v>11448546280.342411</v>
       </c>
-      <c r="AR106" s="45">
+      <c r="AR106" s="39">
         <f t="shared" si="17"/>
         <v>11984478571.839155</v>
       </c>
-      <c r="AS106" s="46" t="s">
+      <c r="AS106" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="AT106" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="AT106" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="AU106" s="48">
+      <c r="AU106" s="42">
         <f>(SUM(AN4:AR4)/5)</f>
         <v>4.6812257065070376E-2</v>
       </c>
@@ -16076,150 +16510,151 @@
       <c r="AK107" s="13"/>
       <c r="AL107" s="13"/>
       <c r="AM107" s="13"/>
-      <c r="AN107" s="46"/>
-      <c r="AO107" s="46"/>
-      <c r="AP107" s="46"/>
-      <c r="AQ107" s="46"/>
-      <c r="AR107" s="49">
+      <c r="AN107" s="40"/>
+      <c r="AO107" s="40"/>
+      <c r="AP107" s="40"/>
+      <c r="AQ107" s="40"/>
+      <c r="AR107" s="43">
         <f>AR106*(1+AU107)/(AU108-AU107)</f>
-        <v>368279628440.29791</v>
-      </c>
-      <c r="AS107" s="50" t="s">
+        <v>365100478040.73871</v>
+      </c>
+      <c r="AS107" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="AT107" s="45" t="s">
         <v>149</v>
       </c>
-      <c r="AT107" s="51" t="s">
-        <v>150</v>
-      </c>
-      <c r="AU107" s="52">
+      <c r="AU107" s="46">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="108" spans="1:47" ht="19" x14ac:dyDescent="0.25">
-      <c r="AN108" s="49">
+      <c r="AN108" s="43">
         <f t="shared" ref="AN108:AP108" si="18">AN107+AN106</f>
         <v>9980308058.8583813</v>
       </c>
-      <c r="AO108" s="49">
+      <c r="AO108" s="43">
         <f t="shared" si="18"/>
         <v>10447508805.298254</v>
       </c>
-      <c r="AP108" s="49">
+      <c r="AP108" s="43">
         <f t="shared" si="18"/>
         <v>10936580273.181463</v>
       </c>
-      <c r="AQ108" s="49">
+      <c r="AQ108" s="43">
         <f>AQ107+AQ106</f>
         <v>11448546280.342411</v>
       </c>
-      <c r="AR108" s="49">
+      <c r="AR108" s="43">
         <f>AR107+AR106</f>
-        <v>380264107012.13708</v>
-      </c>
-      <c r="AS108" s="50" t="s">
-        <v>145</v>
-      </c>
-      <c r="AT108" s="53" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU108" s="54">
+        <v>377084956612.57788</v>
+      </c>
+      <c r="AS108" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="AT108" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="AU108" s="48">
         <f>AU105</f>
-        <v>5.835533542313899E-2</v>
+        <v>5.864578047680466E-2</v>
       </c>
     </row>
     <row r="109" spans="1:47" ht="19" x14ac:dyDescent="0.25">
-      <c r="AN109" s="55" t="s">
-        <v>152</v>
-      </c>
-      <c r="AO109" s="56"/>
+      <c r="AN109" s="60" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO109" s="61"/>
     </row>
     <row r="110" spans="1:47" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN110" s="57" t="s">
-        <v>153</v>
-      </c>
-      <c r="AO110" s="58">
+      <c r="AN110" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="AO110" s="50">
         <f>NPV(AU108,AN108,AO108,AP108,AQ108,AR108)</f>
-        <v>323477638387.32666</v>
+        <v>320668833241.29193</v>
       </c>
     </row>
     <row r="111" spans="1:47" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN111" s="57" t="s">
-        <v>154</v>
-      </c>
-      <c r="AO111" s="58">
+      <c r="AN111" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="AO111" s="50">
         <f>AM40</f>
         <v>11631000000</v>
       </c>
     </row>
     <row r="112" spans="1:47" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN112" s="57" t="s">
-        <v>141</v>
-      </c>
-      <c r="AO112" s="58">
+      <c r="AN112" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="AO112" s="50">
         <f>AU99</f>
         <v>39149000000</v>
       </c>
     </row>
     <row r="113" spans="40:41" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN113" s="57" t="s">
-        <v>155</v>
-      </c>
-      <c r="AO113" s="58">
+      <c r="AN113" s="49" t="s">
+        <v>154</v>
+      </c>
+      <c r="AO113" s="50">
         <f>AO110+AO111-AO112</f>
-        <v>295959638387.32666</v>
+        <v>293150833241.29193</v>
       </c>
     </row>
     <row r="114" spans="40:41" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN114" s="57" t="s">
-        <v>156</v>
-      </c>
-      <c r="AO114" s="59">
+      <c r="AN114" s="49" t="s">
+        <v>155</v>
+      </c>
+      <c r="AO114" s="51">
         <f>AM34*(1+(5*AS16))</f>
         <v>4322108298.1662579</v>
       </c>
     </row>
     <row r="115" spans="40:41" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN115" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="AO115" s="61">
+      <c r="AN115" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="AO115" s="53">
         <f>AO113/AO114</f>
-        <v>68.475757193056353</v>
+        <v>67.825887973623225</v>
       </c>
     </row>
     <row r="116" spans="40:41" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN116" s="62" t="s">
-        <v>158</v>
-      </c>
-      <c r="AO116" s="63">
-        <v>61.86</v>
+      <c r="AN116" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="AO116" s="59" cm="1">
+        <f t="array" ref="AO116">_FV(A1,"Price")</f>
+        <v>62.84</v>
       </c>
     </row>
     <row r="117" spans="40:41" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN117" s="64" t="s">
-        <v>159</v>
-      </c>
-      <c r="AO117" s="65">
+      <c r="AN117" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="AO117" s="55">
         <f>AO115/AO116-1</f>
-        <v>0.10694725497989577</v>
+        <v>7.9342583921439003E-2</v>
       </c>
     </row>
     <row r="118" spans="40:41" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN118" s="64" t="s">
-        <v>160</v>
-      </c>
-      <c r="AO118" s="66" t="str">
+      <c r="AN118" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="AO118" s="56" t="str">
         <f>IF(AO115&gt;AO116,"BUY","SELL")</f>
         <v>BUY</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="AN109:AO109"/>
     <mergeCell ref="AT83:AU83"/>
     <mergeCell ref="AT84:AU84"/>
     <mergeCell ref="AT93:AU93"/>
     <mergeCell ref="AT98:AU98"/>
     <mergeCell ref="AT104:AU104"/>
-    <mergeCell ref="AN109:AO109"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" tooltip="https://roic.ai/company/KO" display="ROIC.AI | KO" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>